<commit_message>
Rewrite to cog part 1
</commit_message>
<xml_diff>
--- a/config/kingdom_queries.xlsx
+++ b/config/kingdom_queries.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -475,7 +475,7 @@
       <c r="A2" s="1" t="inlineStr"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>TWO</t>
+          <t>Two</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -486,7 +486,7 @@
       <c r="A3" s="1" t="n"/>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>THREE</t>
+          <t>Three</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -497,7 +497,7 @@
       <c r="A4" s="1" t="n"/>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>FOUR</t>
+          <t>Four</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -508,7 +508,7 @@
       <c r="A5" s="1" t="n"/>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>FIVE</t>
+          <t>Five</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -519,7 +519,7 @@
       <c r="A6" s="1" t="n"/>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>OTHER</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -529,12 +529,12 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>ACTION</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>TWO</t>
+          <t>Two</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -545,7 +545,7 @@
       <c r="A8" s="1" t="n"/>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>THREE</t>
+          <t>Three</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -556,7 +556,7 @@
       <c r="A9" s="1" t="n"/>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>FOUR</t>
+          <t>Four</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -567,7 +567,7 @@
       <c r="A10" s="1" t="n"/>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>FIVE</t>
+          <t>Five</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -578,7 +578,7 @@
       <c r="A11" s="1" t="n"/>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>OTHER</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -588,12 +588,12 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>ACTION - ATTACK</t>
+          <t>Action - Attack</t>
         </is>
       </c>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>TWO</t>
+          <t>Two</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -604,7 +604,7 @@
       <c r="A13" s="1" t="n"/>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>THREE</t>
+          <t>Three</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -615,7 +615,7 @@
       <c r="A14" s="1" t="n"/>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>FOUR</t>
+          <t>Four</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -626,7 +626,7 @@
       <c r="A15" s="1" t="n"/>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>FIVE</t>
+          <t>Five</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -637,7 +637,7 @@
       <c r="A16" s="1" t="n"/>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>OTHER</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -647,12 +647,12 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>ACTION - ATTACK - DOOM</t>
+          <t>Action - Attack - Doom</t>
         </is>
       </c>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>FOUR</t>
+          <t>Four</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -663,7 +663,7 @@
       <c r="A18" s="1" t="n"/>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>FIVE</t>
+          <t>Five</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -673,12 +673,12 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>ACTION - ATTACK - DURATION</t>
+          <t>Action - Attack - Duration</t>
         </is>
       </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>THREE</t>
+          <t>Three</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -689,7 +689,7 @@
       <c r="A20" s="1" t="n"/>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>FOUR</t>
+          <t>Four</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -700,7 +700,7 @@
       <c r="A21" s="1" t="n"/>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>FIVE</t>
+          <t>Five</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -711,7 +711,7 @@
       <c r="A22" s="1" t="n"/>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>OTHER</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -721,12 +721,12 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>ACTION - ATTACK - DURATION - LOOT</t>
+          <t>Action - Attack - Duration - Loot</t>
         </is>
       </c>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>FIVE</t>
+          <t>Five</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -736,12 +736,12 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>ACTION - ATTACK - LOOTER</t>
+          <t>Action - Attack - Looter</t>
         </is>
       </c>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>FOUR</t>
+          <t>Four</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -752,7 +752,7 @@
       <c r="A25" s="1" t="n"/>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>FIVE</t>
+          <t>Five</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -762,12 +762,12 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>ACTION - ATTACK - OMEN</t>
+          <t>Action - Attack - Omen</t>
         </is>
       </c>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>FIVE</t>
+          <t>Five</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -777,12 +777,12 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>ACTION - DOOM</t>
+          <t>Action - Doom</t>
         </is>
       </c>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>THREE</t>
+          <t>Three</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -793,7 +793,7 @@
       <c r="A28" s="1" t="n"/>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>FIVE</t>
+          <t>Five</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -803,12 +803,12 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>ACTION - DURATION</t>
+          <t>Action - Duration</t>
         </is>
       </c>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>TWO</t>
+          <t>Two</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -819,7 +819,7 @@
       <c r="A30" s="1" t="n"/>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>THREE</t>
+          <t>Three</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -830,7 +830,7 @@
       <c r="A31" s="1" t="n"/>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>FOUR</t>
+          <t>Four</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -841,7 +841,7 @@
       <c r="A32" s="1" t="n"/>
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>FIVE</t>
+          <t>Five</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -852,7 +852,7 @@
       <c r="A33" s="1" t="n"/>
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>OTHER</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -862,12 +862,12 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>ACTION - DURATION - LIAISON</t>
+          <t>Action - Duration - Liaison</t>
         </is>
       </c>
       <c r="B34" s="1" t="inlineStr">
         <is>
-          <t>THREE</t>
+          <t>Three</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -877,12 +877,12 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>ACTION - DURATION - LOOT</t>
+          <t>Action - Duration - Loot</t>
         </is>
       </c>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>TWO</t>
+          <t>Two</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -892,12 +892,12 @@
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>ACTION - FATE</t>
+          <t>Action - Fate</t>
         </is>
       </c>
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>TWO</t>
+          <t>Two</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -908,7 +908,7 @@
       <c r="A37" s="1" t="n"/>
       <c r="B37" s="1" t="inlineStr">
         <is>
-          <t>THREE</t>
+          <t>Three</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -919,7 +919,7 @@
       <c r="A38" s="1" t="n"/>
       <c r="B38" s="1" t="inlineStr">
         <is>
-          <t>FOUR</t>
+          <t>Four</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -930,7 +930,7 @@
       <c r="A39" s="1" t="n"/>
       <c r="B39" s="1" t="inlineStr">
         <is>
-          <t>FIVE</t>
+          <t>Five</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -940,12 +940,12 @@
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>ACTION - LIAISON</t>
+          <t>Action - Liaison</t>
         </is>
       </c>
       <c r="B40" s="1" t="inlineStr">
         <is>
-          <t>TWO</t>
+          <t>Two</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -956,7 +956,7 @@
       <c r="A41" s="1" t="n"/>
       <c r="B41" s="1" t="inlineStr">
         <is>
-          <t>THREE</t>
+          <t>Three</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -967,7 +967,7 @@
       <c r="A42" s="1" t="n"/>
       <c r="B42" s="1" t="inlineStr">
         <is>
-          <t>FOUR</t>
+          <t>Four</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -978,7 +978,7 @@
       <c r="A43" s="1" t="n"/>
       <c r="B43" s="1" t="inlineStr">
         <is>
-          <t>FIVE</t>
+          <t>Five</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -988,12 +988,12 @@
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>ACTION - LOOT</t>
+          <t>Action - Loot</t>
         </is>
       </c>
       <c r="B44" s="1" t="inlineStr">
         <is>
-          <t>FIVE</t>
+          <t>Five</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1003,12 +1003,12 @@
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>ACTION - LOOTER</t>
+          <t>Action - Looter</t>
         </is>
       </c>
       <c r="B45" s="1" t="inlineStr">
         <is>
-          <t>FOUR</t>
+          <t>Four</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1018,12 +1018,12 @@
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>ACTION - OMEN</t>
+          <t>Action - Omen</t>
         </is>
       </c>
       <c r="B46" s="1" t="inlineStr">
         <is>
-          <t>FOUR</t>
+          <t>Four</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1034,7 +1034,7 @@
       <c r="A47" s="1" t="n"/>
       <c r="B47" s="1" t="inlineStr">
         <is>
-          <t>FIVE</t>
+          <t>Five</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1045,7 +1045,7 @@
       <c r="A48" s="1" t="n"/>
       <c r="B48" s="1" t="inlineStr">
         <is>
-          <t>OTHER</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1055,12 +1055,12 @@
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>ACTION - TREASURE</t>
+          <t>Action - Treasure</t>
         </is>
       </c>
       <c r="B49" s="1" t="inlineStr">
         <is>
-          <t>FIVE</t>
+          <t>Five</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1070,12 +1070,12 @@
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>ATTACK - DOOM</t>
+          <t>Attack - Doom</t>
         </is>
       </c>
       <c r="B50" s="1" t="inlineStr">
         <is>
-          <t>FIVE</t>
+          <t>Five</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -1085,12 +1085,12 @@
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>ATTACK - DURATION</t>
+          <t>Attack - Duration</t>
         </is>
       </c>
       <c r="B51" s="1" t="inlineStr">
         <is>
-          <t>OTHER</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1100,12 +1100,12 @@
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>ATTACK - FATE - TREASURE</t>
+          <t>Attack - Fate - Treasure</t>
         </is>
       </c>
       <c r="B52" s="1" t="inlineStr">
         <is>
-          <t>FIVE</t>
+          <t>Five</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1115,12 +1115,12 @@
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>ATTACK - TREASURE</t>
+          <t>Attack - Treasure</t>
         </is>
       </c>
       <c r="B53" s="1" t="inlineStr">
         <is>
-          <t>FIVE</t>
+          <t>Five</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1130,12 +1130,12 @@
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>DURATION</t>
+          <t>Duration</t>
         </is>
       </c>
       <c r="B54" s="1" t="inlineStr">
         <is>
-          <t>TWO</t>
+          <t>Two</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -1146,7 +1146,7 @@
       <c r="A55" s="1" t="n"/>
       <c r="B55" s="1" t="inlineStr">
         <is>
-          <t>THREE</t>
+          <t>Three</t>
         </is>
       </c>
       <c r="C55" t="n">
@@ -1157,7 +1157,7 @@
       <c r="A56" s="1" t="n"/>
       <c r="B56" s="1" t="inlineStr">
         <is>
-          <t>FIVE</t>
+          <t>Five</t>
         </is>
       </c>
       <c r="C56" t="n">
@@ -1167,12 +1167,12 @@
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>DURATION - LIAISON - TREASURE</t>
+          <t>Duration - Liaison - Treasure</t>
         </is>
       </c>
       <c r="B57" s="1" t="inlineStr">
         <is>
-          <t>FIVE</t>
+          <t>Five</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -1182,12 +1182,12 @@
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>DURATION - TREASURE</t>
+          <t>Duration - Treasure</t>
         </is>
       </c>
       <c r="B58" s="1" t="inlineStr">
         <is>
-          <t>TWO</t>
+          <t>Two</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -1198,7 +1198,7 @@
       <c r="A59" s="1" t="n"/>
       <c r="B59" s="1" t="inlineStr">
         <is>
-          <t>THREE</t>
+          <t>Three</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -1209,7 +1209,7 @@
       <c r="A60" s="1" t="n"/>
       <c r="B60" s="1" t="inlineStr">
         <is>
-          <t>FOUR</t>
+          <t>Four</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -1220,7 +1220,7 @@
       <c r="A61" s="1" t="n"/>
       <c r="B61" s="1" t="inlineStr">
         <is>
-          <t>FIVE</t>
+          <t>Five</t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -1230,12 +1230,12 @@
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>LIAISON - TREASURE</t>
+          <t>Liaison - Treasure</t>
         </is>
       </c>
       <c r="B62" s="1" t="inlineStr">
         <is>
-          <t>TWO</t>
+          <t>Two</t>
         </is>
       </c>
       <c r="C62" t="n">
@@ -1245,12 +1245,12 @@
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>LOOT - TREASURE</t>
+          <t>Loot - Treasure</t>
         </is>
       </c>
       <c r="B63" s="1" t="inlineStr">
         <is>
-          <t>TWO</t>
+          <t>Two</t>
         </is>
       </c>
       <c r="C63" t="n">
@@ -1261,7 +1261,7 @@
       <c r="A64" s="1" t="n"/>
       <c r="B64" s="1" t="inlineStr">
         <is>
-          <t>FIVE</t>
+          <t>Five</t>
         </is>
       </c>
       <c r="C64" t="n">
@@ -1272,7 +1272,7 @@
       <c r="A65" s="1" t="n"/>
       <c r="B65" s="1" t="inlineStr">
         <is>
-          <t>OTHER</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -1282,12 +1282,12 @@
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>TREASURE</t>
+          <t>Treasure</t>
         </is>
       </c>
       <c r="B66" s="1" t="inlineStr">
         <is>
-          <t>TWO</t>
+          <t>Two</t>
         </is>
       </c>
       <c r="C66" t="n">
@@ -1298,7 +1298,7 @@
       <c r="A67" s="1" t="n"/>
       <c r="B67" s="1" t="inlineStr">
         <is>
-          <t>THREE</t>
+          <t>Three</t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -1309,7 +1309,7 @@
       <c r="A68" s="1" t="n"/>
       <c r="B68" s="1" t="inlineStr">
         <is>
-          <t>FOUR</t>
+          <t>Four</t>
         </is>
       </c>
       <c r="C68" t="n">
@@ -1320,7 +1320,7 @@
       <c r="A69" s="1" t="n"/>
       <c r="B69" s="1" t="inlineStr">
         <is>
-          <t>FIVE</t>
+          <t>Five</t>
         </is>
       </c>
       <c r="C69" t="n">
@@ -1331,7 +1331,7 @@
       <c r="A70" s="1" t="n"/>
       <c r="B70" s="1" t="inlineStr">
         <is>
-          <t>OTHER</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="C70" t="n">

</xml_diff>